<commit_message>
modularisation and R package built
</commit_message>
<xml_diff>
--- a/Validation/2022-09-04 reads/example1.xlsx
+++ b/Validation/2022-09-04 reads/example1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markc\Dropbox (Cambridge University)\temp\NormaliseForIC50\Validation\2022-09-04 reads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65753C6E-B58A-43E4-963B-7EDE0E03D2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E861A149-AE6F-46B3-8D99-7DEE74068B32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="138">
   <si>
     <t>Result: mc sda111</t>
   </si>
@@ -450,6 +450,12 @@
   </si>
   <si>
     <t>Result: mc example1</t>
+  </si>
+  <si>
+    <t>neg</t>
+  </si>
+  <si>
+    <t>pos</t>
   </si>
 </sst>
 </file>
@@ -1470,7 +1476,7 @@
   <dimension ref="A1:Q23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1573,11 +1579,11 @@
       <c r="D10" s="13">
         <v>1</v>
       </c>
-      <c r="F10" s="12">
-        <v>1</v>
-      </c>
-      <c r="G10" s="12">
-        <v>2</v>
+      <c r="F10" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>137</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>132</v>

</xml_diff>